<commit_message>
excel adding branch4 original
</commit_message>
<xml_diff>
--- a/Test branch.xlsx
+++ b/Test branch.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tripti Mehta\Desktop\Industry Connect\GitHubRepository\ProjectMarsQA2\ProjectMarsQA2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D4BC93-A768-4D15-B2D9-47C3D1132164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058178F8-263E-4E25-A849-0D029258FAE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{E9F7D5A9-FBFA-49C3-BA4D-0DAA99558B5A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{E9F7D5A9-FBFA-49C3-BA4D-0DAA99558B5A}"/>
   </bookViews>
   <sheets>
     <sheet name="branch2" sheetId="1" r:id="rId1"/>
     <sheet name="branch4" sheetId="2" r:id="rId2"/>
+    <sheet name="branch4 original" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
   <si>
     <t>Use cases</t>
   </si>
@@ -140,13 +141,67 @@
   </si>
   <si>
     <t>Existing user cancelling updating language with valid credentials</t>
+  </si>
+  <si>
+    <t>Test Cases</t>
+  </si>
+  <si>
+    <t>Verify if an existing user is able to login to Mars with valid email address and password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify if user is taken to their home page upon login in to Mars successfully with valid credentials </t>
+  </si>
+  <si>
+    <t>Verify if a new user is able to register to Mars using the register functionality</t>
+  </si>
+  <si>
+    <t>Verify if an existing user is not allowed to login to Mars with valid email address and invalid password</t>
+  </si>
+  <si>
+    <t>Verify if an existing user is not allowed to login to mars with invalid email address and valid password</t>
+  </si>
+  <si>
+    <t>Verify if an existing user is not allowed to login to Mars with invalid email address and invalid password</t>
+  </si>
+  <si>
+    <t>Verify if an existing user is not allowed to login to Mars with null email address and a valid password</t>
+  </si>
+  <si>
+    <t>Verify if an existing user is not allowed to login to Mars with valid email address and null password</t>
+  </si>
+  <si>
+    <t>Verify if an existing user is not allowed to login to Mars with null email address and null password</t>
+  </si>
+  <si>
+    <t>Verify if an existing user is not allowed to login to Mars with null email address and invalid password</t>
+  </si>
+  <si>
+    <t>Verify if an existing user is not allowed to login to Mars with invalid email address and null password</t>
+  </si>
+  <si>
+    <t>Verify if an existing user is not allowed to see other user's home page upon login</t>
+  </si>
+  <si>
+    <t>Verify new user is able to add a language</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify existing user is able to add a language </t>
+  </si>
+  <si>
+    <t>Verify new user is able to delete a language</t>
+  </si>
+  <si>
+    <t>Verify existing user is able to delete a language</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify new user is able to update a language </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,8 +209,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -168,8 +236,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF999999"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -177,11 +257,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -199,6 +294,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -623,8 +729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE1E672C-BF3F-4D54-8124-9616CFC35D56}">
   <dimension ref="A1:A21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -740,4 +846,112 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4E42BF6-8CDE-4A59-9487-D9EFD3B46AC9}">
+  <dimension ref="A1:A18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="65" style="7" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="26" x14ac:dyDescent="0.35">
+      <c r="A2" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="26" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="26" x14ac:dyDescent="0.35">
+      <c r="A5" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="26" x14ac:dyDescent="0.35">
+      <c r="A6" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="26" x14ac:dyDescent="0.35">
+      <c r="A7" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="26" x14ac:dyDescent="0.35">
+      <c r="A8" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="26" x14ac:dyDescent="0.35">
+      <c r="A9" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="26" x14ac:dyDescent="0.35">
+      <c r="A10" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="26" x14ac:dyDescent="0.35">
+      <c r="A11" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="26" x14ac:dyDescent="0.35">
+      <c r="A12" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="26" x14ac:dyDescent="0.35">
+      <c r="A13" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>